<commit_message>
Upgrade Apache POI to version 4.1.1
Adapt code to not use a deprecated constructor anymore.

Signed-off-by: Sebastian Schuberth <sebastian.schuberth@bosch-si.com>
</commit_message>
<xml_diff>
--- a/reporter/src/funTest/assets/file-counter-expected-scan-report.xlsx
+++ b/reporter/src/funTest/assets/file-counter-expected-scan-report.xlsx
@@ -1,31 +1,6 @@
-
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\oss-review-toolkit\reporter\src\funTest\assets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE983D5-6EC4-447C-B410-CB015A7F3757}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="2250" yWindow="1365" windowWidth="33120" windowHeight="17955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Gradle com.here.ort.gradle.exam" sheetId="2" r:id="rId2"/>
-  </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Gradle com.here.ort.gradle.exam'!$A$10:$F$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$A$10:$F$15</definedName>
-  </definedNames>
-  <calcPr calcId="0"/>
-</workbook>
-</file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="38">
   <si>
     <t>Project:</t>
   </si>
@@ -256,6 +231,15 @@
 Suppressed: DownloadException: No VCS URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'. Please make sure the release POM file includes the SCM connection, see: https://docs.gradle.org/current/userguide/publishing_maven.html#example_customizing_the_pom_file, 
 Suppressed: DownloadException: No source artifact URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'.
 </t>
+  </si>
+  <si>
+    <t>EPL-1.0</t>
+  </si>
+  <si>
+    <t>Apache-2.0</t>
+  </si>
+  <si>
+    <t>BSD-3-Clause</t>
   </si>
 </sst>
 </file>
@@ -325,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -339,14 +323,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -659,466 +646,4 @@
     </a:ext>
   </a:extLst>
 </a:theme>
-</file>
-
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="254.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1">
-      <c r="A11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="45" customHeight="1">
-      <c r="A12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="75" customHeight="1">
-      <c r="A13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="75" customHeight="1">
-      <c r="A14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="45" customHeight="1">
-      <c r="A15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A10:F15" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="6">
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="254.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1">
-      <c r="A11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1">
-      <c r="A12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" customHeight="1">
-      <c r="A13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1">
-      <c r="A14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1">
-      <c r="A15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A10:F15" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <mergeCells count="6">
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>